<commit_message>
Improved some column handling, added identifiers and experimental data to output
</commit_message>
<xml_diff>
--- a/Output/QSAR_predictions_explained.xlsx
+++ b/Output/QSAR_predictions_explained.xlsx
@@ -8,12 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\QSAR_predictions_database\Output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B6FEFE7-F910-42AB-9C20-9FE350606A87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C896D36-2D30-449C-B8A9-3DA61151F2E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{2D05DBB1-4549-420F-9A87-95D458EF22FE}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" activeTab="2" xr2:uid="{2D05DBB1-4549-420F-9A87-95D458EF22FE}"/>
   </bookViews>
   <sheets>
-    <sheet name="Column names" sheetId="1" r:id="rId1"/>
+    <sheet name="info" sheetId="4" r:id="rId1"/>
+    <sheet name="QSAR_predictions_v11 cols" sheetId="1" r:id="rId2"/>
+    <sheet name="experimental_dataset_v11 cols" sheetId="2" r:id="rId3"/>
+    <sheet name="identifiers_v11 cols" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2408" uniqueCount="660">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3144" uniqueCount="1019">
   <si>
     <t>META_QSARn</t>
   </si>
@@ -2015,14 +2018,1091 @@
     <t>TEST consensus prediction acute fish</t>
   </si>
   <si>
-    <t xml:space="preserve">Explanation of column contents in </t>
+    <t>This excel-file explains the output files of the QSAR-predictions_database project</t>
+  </si>
+  <si>
+    <t>Contents:</t>
+  </si>
+  <si>
+    <t>info sheet</t>
+  </si>
+  <si>
+    <t>QSAR_predictions_v11 cols</t>
+  </si>
+  <si>
+    <t>experimental_dataset_v11 cols</t>
+  </si>
+  <si>
+    <t>identifiers_v11 cols</t>
+  </si>
+  <si>
+    <t>Descriptions of the column contents of the QSAR predictions file</t>
+  </si>
+  <si>
+    <t>Descriptions of the column contents of the empirical data file</t>
+  </si>
+  <si>
+    <t>Descriptions of the column contents of the chemical identifiers and physicochemical data file</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Project can be found here: </t>
+  </si>
+  <si>
+    <t>https://github.com/ThomasBackhausLab/QSAR_predictions_database</t>
+  </si>
+  <si>
+    <t>original_CAS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">original_SMILES </t>
+  </si>
+  <si>
+    <t>InChIKey</t>
+  </si>
+  <si>
+    <t>CID</t>
+  </si>
+  <si>
+    <t>logkow</t>
+  </si>
+  <si>
+    <t xml:space="preserve">logkow_source </t>
+  </si>
+  <si>
+    <t>pka</t>
+  </si>
+  <si>
+    <t>molecule_number</t>
+  </si>
+  <si>
+    <t>numric</t>
+  </si>
+  <si>
+    <t>Internal identifier used to match QSAR predictions with identifier</t>
+  </si>
+  <si>
+    <t>For any questions, contact patrik.svedberg@bioenv.gu.se</t>
+  </si>
+  <si>
+    <t>This page you are on. Really.</t>
+  </si>
+  <si>
+    <t>original_SMILES</t>
+  </si>
+  <si>
+    <t>Media_type</t>
+  </si>
+  <si>
+    <t>Species_name</t>
+  </si>
+  <si>
+    <t>Duration_hour</t>
+  </si>
+  <si>
+    <t>Conc_mgL</t>
+  </si>
+  <si>
+    <t>Conc_sign</t>
+  </si>
+  <si>
+    <t>Database</t>
+  </si>
+  <si>
+    <t>EFSA_documentReferencePK</t>
+  </si>
+  <si>
+    <t>EFSA_substanceKey</t>
+  </si>
+  <si>
+    <t>EFSA_substanceDesc</t>
+  </si>
+  <si>
+    <t>EFSA_ECNO</t>
+  </si>
+  <si>
+    <t>EFSA_studyName</t>
+  </si>
+  <si>
+    <t>EFSA_endpointKind</t>
+  </si>
+  <si>
+    <t>EFSA_resutType</t>
+  </si>
+  <si>
+    <t>EFSA_reliability</t>
+  </si>
+  <si>
+    <t>EFSA_rationalReliability</t>
+  </si>
+  <si>
+    <t>EFSA_GLPCompliance</t>
+  </si>
+  <si>
+    <t>EFSA_testMaterial</t>
+  </si>
+  <si>
+    <t>EFSA_testMaterialIndicator</t>
+  </si>
+  <si>
+    <t>EFSA_analyticalMonitoring</t>
+  </si>
+  <si>
+    <t>EFSA_vehicle</t>
+  </si>
+  <si>
+    <t>EFSA_testType</t>
+  </si>
+  <si>
+    <t>EFSA_limitTest</t>
+  </si>
+  <si>
+    <t>EFSA_exposureDurationValue</t>
+  </si>
+  <si>
+    <t>EFSA_exposureDurationUnit</t>
+  </si>
+  <si>
+    <t>EFSA_expDurationValue</t>
+  </si>
+  <si>
+    <t>EFSA_expDurationUnit</t>
+  </si>
+  <si>
+    <t>EFSA_minValue</t>
+  </si>
+  <si>
+    <t>EFSA_endpointUnit</t>
+  </si>
+  <si>
+    <t>EFSA_basisConc</t>
+  </si>
+  <si>
+    <t>EFSA_effectConcType</t>
+  </si>
+  <si>
+    <t>EFSA_basisEffect</t>
+  </si>
+  <si>
+    <t>EFSA_remarks</t>
+  </si>
+  <si>
+    <t>EFSA_species_group</t>
+  </si>
+  <si>
+    <t>ECOTOX_obs_duration_unit</t>
+  </si>
+  <si>
+    <t>ECOTOX_exposure_duration_unit</t>
+  </si>
+  <si>
+    <t>ECOTOX_study_duration_unit</t>
+  </si>
+  <si>
+    <t>ECOTOX_organism_age_unit</t>
+  </si>
+  <si>
+    <t>ECOTOX_measurement_code</t>
+  </si>
+  <si>
+    <t>ECOTOX_endpoint_code</t>
+  </si>
+  <si>
+    <t>ECOTOX_effect_code</t>
+  </si>
+  <si>
+    <t>ECOTOX_species_number</t>
+  </si>
+  <si>
+    <t>ECOTOX_reference_number</t>
+  </si>
+  <si>
+    <t>ECOTOX_test_id</t>
+  </si>
+  <si>
+    <t>ECOTOX_result_id</t>
+  </si>
+  <si>
+    <t>ECOTOX_sample_size_mean_op</t>
+  </si>
+  <si>
+    <t>ECOTOX_sample_size_mean</t>
+  </si>
+  <si>
+    <t>ECOTOX_sample_size_min_op</t>
+  </si>
+  <si>
+    <t>ECOTOX_sample_size_min</t>
+  </si>
+  <si>
+    <t>ECOTOX_sample_size_max_op</t>
+  </si>
+  <si>
+    <t>ECOTOX_sample_size_max</t>
+  </si>
+  <si>
+    <t>ECOTOX_sample_size_unit</t>
+  </si>
+  <si>
+    <t>ECOTOX_sample_size_comments</t>
+  </si>
+  <si>
+    <t>ECOTOX_obs_duration_mean_op</t>
+  </si>
+  <si>
+    <t>ECOTOX_obs_duration_mean</t>
+  </si>
+  <si>
+    <t>ECOTOX_obs_duration_min_op</t>
+  </si>
+  <si>
+    <t>ECOTOX_obs_duration_min</t>
+  </si>
+  <si>
+    <t>ECOTOX_obs_duration_max_op</t>
+  </si>
+  <si>
+    <t>ECOTOX_obs_duration_max</t>
+  </si>
+  <si>
+    <t>ECOTOX_obs_duration_comments</t>
+  </si>
+  <si>
+    <t>ECOTOX_endpoint_comments</t>
+  </si>
+  <si>
+    <t>ECOTOX_trend</t>
+  </si>
+  <si>
+    <t>ECOTOX_effect</t>
+  </si>
+  <si>
+    <t>ECOTOX_effect_comments</t>
+  </si>
+  <si>
+    <t>ECOTOX_measurement</t>
+  </si>
+  <si>
+    <t>ECOTOX_measurement_comments</t>
+  </si>
+  <si>
+    <t>ECOTOX_response_site</t>
+  </si>
+  <si>
+    <t>ECOTOX_response_site_comments</t>
+  </si>
+  <si>
+    <t>ECOTOX_effect_pct_mean_op</t>
+  </si>
+  <si>
+    <t>ECOTOX_effect_pct_mean</t>
+  </si>
+  <si>
+    <t>ECOTOX_effect_pct_min_op</t>
+  </si>
+  <si>
+    <t>ECOTOX_effect_pct_min</t>
+  </si>
+  <si>
+    <t>ECOTOX_effect_pct_max_op</t>
+  </si>
+  <si>
+    <t>ECOTOX_effect_pct_max</t>
+  </si>
+  <si>
+    <t>ECOTOX_effect_pct_comments</t>
+  </si>
+  <si>
+    <t>ECOTOX_conc1_type</t>
+  </si>
+  <si>
+    <t>ECOTOX_ion1</t>
+  </si>
+  <si>
+    <t>ECOTOX_conc1_mean</t>
+  </si>
+  <si>
+    <t>ECOTOX_conc1_min_op</t>
+  </si>
+  <si>
+    <t>ECOTOX_conc1_min</t>
+  </si>
+  <si>
+    <t>ECOTOX_conc1_max_op</t>
+  </si>
+  <si>
+    <t>ECOTOX_conc1_max</t>
+  </si>
+  <si>
+    <t>ECOTOX_conc1_unit</t>
+  </si>
+  <si>
+    <t>ECOTOX_conc1_comments</t>
+  </si>
+  <si>
+    <t>ECOTOX_conc2_type</t>
+  </si>
+  <si>
+    <t>ECOTOX_ion2</t>
+  </si>
+  <si>
+    <t>ECOTOX_conc2_mean_op</t>
+  </si>
+  <si>
+    <t>ECOTOX_conc2_mean</t>
+  </si>
+  <si>
+    <t>ECOTOX_conc2_min_op</t>
+  </si>
+  <si>
+    <t>ECOTOX_conc2_min</t>
+  </si>
+  <si>
+    <t>ECOTOX_conc2_max_op</t>
+  </si>
+  <si>
+    <t>ECOTOX_conc2_max</t>
+  </si>
+  <si>
+    <t>ECOTOX_conc2_unit</t>
+  </si>
+  <si>
+    <t>ECOTOX_conc2_comments</t>
+  </si>
+  <si>
+    <t>ECOTOX_conc3_type</t>
+  </si>
+  <si>
+    <t>ECOTOX_ion3</t>
+  </si>
+  <si>
+    <t>ECOTOX_conc3_mean_op</t>
+  </si>
+  <si>
+    <t>ECOTOX_conc3_mean</t>
+  </si>
+  <si>
+    <t>ECOTOX_conc3_min_op</t>
+  </si>
+  <si>
+    <t>ECOTOX_conc3_min</t>
+  </si>
+  <si>
+    <t>ECOTOX_conc3_max_op</t>
+  </si>
+  <si>
+    <t>ECOTOX_conc3_max</t>
+  </si>
+  <si>
+    <t>ECOTOX_conc3_unit</t>
+  </si>
+  <si>
+    <t>ECOTOX_conc3_comments</t>
+  </si>
+  <si>
+    <t>ECOTOX_bcf1_mean_op</t>
+  </si>
+  <si>
+    <t>ECOTOX_bcf1_mean</t>
+  </si>
+  <si>
+    <t>ECOTOX_bcf1_min_op</t>
+  </si>
+  <si>
+    <t>ECOTOX_bcf1_min</t>
+  </si>
+  <si>
+    <t>ECOTOX_bcf1_max_op</t>
+  </si>
+  <si>
+    <t>ECOTOX_bcf1_max</t>
+  </si>
+  <si>
+    <t>ECOTOX_bcf1_unit</t>
+  </si>
+  <si>
+    <t>ECOTOX_bcf1_comments</t>
+  </si>
+  <si>
+    <t>ECOTOX_bcf2_mean_op</t>
+  </si>
+  <si>
+    <t>ECOTOX_bcf2_mean</t>
+  </si>
+  <si>
+    <t>ECOTOX_bcf2_min_op</t>
+  </si>
+  <si>
+    <t>ECOTOX_bcf2_min</t>
+  </si>
+  <si>
+    <t>ECOTOX_bcf2_max_op</t>
+  </si>
+  <si>
+    <t>ECOTOX_bcf2_max</t>
+  </si>
+  <si>
+    <t>ECOTOX_bcf2_unit</t>
+  </si>
+  <si>
+    <t>ECOTOX_bcf2_comments</t>
+  </si>
+  <si>
+    <t>ECOTOX_bcf3_mean_op</t>
+  </si>
+  <si>
+    <t>ECOTOX_bcf3_mean</t>
+  </si>
+  <si>
+    <t>ECOTOX_bcf3_min_op</t>
+  </si>
+  <si>
+    <t>ECOTOX_bcf3_min</t>
+  </si>
+  <si>
+    <t>ECOTOX_bcf3_max_op</t>
+  </si>
+  <si>
+    <t>ECOTOX_bcf3_max</t>
+  </si>
+  <si>
+    <t>ECOTOX_bcf3_unit</t>
+  </si>
+  <si>
+    <t>ECOTOX_bcf3_comments</t>
+  </si>
+  <si>
+    <t>ECOTOX_significance_code</t>
+  </si>
+  <si>
+    <t>ECOTOX_significance_type</t>
+  </si>
+  <si>
+    <t>ECOTOX_significance_level_mean_op</t>
+  </si>
+  <si>
+    <t>ECOTOX_significance_level_mean</t>
+  </si>
+  <si>
+    <t>ECOTOX_significance_level_min_op</t>
+  </si>
+  <si>
+    <t>ECOTOX_significance_level_min</t>
+  </si>
+  <si>
+    <t>ECOTOX_significance_level_max_op</t>
+  </si>
+  <si>
+    <t>ECOTOX_significance_level_max</t>
+  </si>
+  <si>
+    <t>ECOTOX_significance_comments</t>
+  </si>
+  <si>
+    <t>ECOTOX_chem_analysis_method</t>
+  </si>
+  <si>
+    <t>ECOTOX_chem_analysis_method_comments</t>
+  </si>
+  <si>
+    <t>ECOTOX_endpoint_assigned</t>
+  </si>
+  <si>
+    <t>ECOTOX_organism_final_wt_mean_op</t>
+  </si>
+  <si>
+    <t>ECOTOX_organism_final_wt_mean</t>
+  </si>
+  <si>
+    <t>ECOTOX_organism_final_wt_min_op</t>
+  </si>
+  <si>
+    <t>ECOTOX_organism_final_wt_min</t>
+  </si>
+  <si>
+    <t>ECOTOX_organism_final_wt_max_op</t>
+  </si>
+  <si>
+    <t>ECOTOX_organism_final_wt_max</t>
+  </si>
+  <si>
+    <t>ECOTOX_organism_final_wt_unit</t>
+  </si>
+  <si>
+    <t>ECOTOX_organism_final_wt_comments</t>
+  </si>
+  <si>
+    <t>ECOTOX_intake_rate_mean_op</t>
+  </si>
+  <si>
+    <t>ECOTOX_intake_rate_mean</t>
+  </si>
+  <si>
+    <t>ECOTOX_intake_rate_min_op</t>
+  </si>
+  <si>
+    <t>ECOTOX_intake_rate_min</t>
+  </si>
+  <si>
+    <t>ECOTOX_intake_rate_max_op</t>
+  </si>
+  <si>
+    <t>ECOTOX_intake_rate_max</t>
+  </si>
+  <si>
+    <t>ECOTOX_intake_rate_unit</t>
+  </si>
+  <si>
+    <t>ECOTOX_intake_rate_comments</t>
+  </si>
+  <si>
+    <t>ECOTOX_lipid_pct_mean_op</t>
+  </si>
+  <si>
+    <t>ECOTOX_lipid_pct_mean</t>
+  </si>
+  <si>
+    <t>ECOTOX_lipid_pct_min_op</t>
+  </si>
+  <si>
+    <t>ECOTOX_lipid_pct_min</t>
+  </si>
+  <si>
+    <t>ECOTOX_lipid_pct_max_op</t>
+  </si>
+  <si>
+    <t>ECOTOX_lipid_pct_max</t>
+  </si>
+  <si>
+    <t>ECOTOX_lipid_pct_comments</t>
+  </si>
+  <si>
+    <t>ECOTOX_dry_wet</t>
+  </si>
+  <si>
+    <t>ECOTOX_dry_wet_pct_mean_op</t>
+  </si>
+  <si>
+    <t>ECOTOX_dry_wet_pct_mean</t>
+  </si>
+  <si>
+    <t>ECOTOX_dry_wet_pct_min_op</t>
+  </si>
+  <si>
+    <t>ECOTOX_dry_wet_pct_min</t>
+  </si>
+  <si>
+    <t>ECOTOX_dry_wet_pct_max_op</t>
+  </si>
+  <si>
+    <t>ECOTOX_dry_wet_pct_max</t>
+  </si>
+  <si>
+    <t>ECOTOX_dry_wet_pct_comments</t>
+  </si>
+  <si>
+    <t>ECOTOX_steady_state</t>
+  </si>
+  <si>
+    <t>ECOTOX_results_additional_comments</t>
+  </si>
+  <si>
+    <t>ECOTOX_companion_tag</t>
+  </si>
+  <si>
+    <t>ECOTOX_results_created_date</t>
+  </si>
+  <si>
+    <t>ECOTOX_results_modified_date</t>
+  </si>
+  <si>
+    <t>ECOTOX_old_terretox_result_number</t>
+  </si>
+  <si>
+    <t>ECOTOX_test_grade</t>
+  </si>
+  <si>
+    <t>ECOTOX_test_grade_comments</t>
+  </si>
+  <si>
+    <t>ECOTOX_test_formulation</t>
+  </si>
+  <si>
+    <t>ECOTOX_test_formulation_comments</t>
+  </si>
+  <si>
+    <t>ECOTOX_test_radiolabel</t>
+  </si>
+  <si>
+    <t>ECOTOX_test_radiolabel_comments</t>
+  </si>
+  <si>
+    <t>ECOTOX_test_purity_mean_op</t>
+  </si>
+  <si>
+    <t>ECOTOX_test_purity_mean</t>
+  </si>
+  <si>
+    <t>ECOTOX_test_purity_min_op</t>
+  </si>
+  <si>
+    <t>ECOTOX_test_purity_min</t>
+  </si>
+  <si>
+    <t>ECOTOX_test_purity_max_op</t>
+  </si>
+  <si>
+    <t>ECOTOX_test_purity_max</t>
+  </si>
+  <si>
+    <t>ECOTOX_test_purity_comments</t>
+  </si>
+  <si>
+    <t>ECOTOX_test_characteristics</t>
+  </si>
+  <si>
+    <t>ECOTOX_organism_habitat</t>
+  </si>
+  <si>
+    <t>ECOTOX_organism_source</t>
+  </si>
+  <si>
+    <t>ECOTOX_organism_source_comments</t>
+  </si>
+  <si>
+    <t>ECOTOX_organism_lifestage</t>
+  </si>
+  <si>
+    <t>ECOTOX_organism_lifestage_comments</t>
+  </si>
+  <si>
+    <t>ECOTOX_organism_age_mean_op</t>
+  </si>
+  <si>
+    <t>ECOTOX_organism_age_mean</t>
+  </si>
+  <si>
+    <t>ECOTOX_organism_age_min_op</t>
+  </si>
+  <si>
+    <t>ECOTOX_organism_age_min</t>
+  </si>
+  <si>
+    <t>ECOTOX_organism_age_max_op</t>
+  </si>
+  <si>
+    <t>ECOTOX_organism_age_max</t>
+  </si>
+  <si>
+    <t>ECOTOX_organism_init_wt_mean_op</t>
+  </si>
+  <si>
+    <t>ECOTOX_organism_init_wt_mean</t>
+  </si>
+  <si>
+    <t>ECOTOX_organism_init_wt_min_op</t>
+  </si>
+  <si>
+    <t>ECOTOX_organism_init_wt_min</t>
+  </si>
+  <si>
+    <t>ECOTOX_organism_init_wt_max_op</t>
+  </si>
+  <si>
+    <t>ECOTOX_organism_init_wt_max</t>
+  </si>
+  <si>
+    <t>ECOTOX_organism_init_wt_unit</t>
+  </si>
+  <si>
+    <t>ECOTOX_organism_characteristics</t>
+  </si>
+  <si>
+    <t>ECOTOX_organism_gender</t>
+  </si>
+  <si>
+    <t>ECOTOX_experimental_design</t>
+  </si>
+  <si>
+    <t>ECOTOX_study_duration_mean_op</t>
+  </si>
+  <si>
+    <t>ECOTOX_study_duration_mean</t>
+  </si>
+  <si>
+    <t>ECOTOX_study_duration_min_op</t>
+  </si>
+  <si>
+    <t>ECOTOX_study_duration_min</t>
+  </si>
+  <si>
+    <t>ECOTOX_study_duration_max_op</t>
+  </si>
+  <si>
+    <t>ECOTOX_study_duration_max</t>
+  </si>
+  <si>
+    <t>ECOTOX_study_duration_comments</t>
+  </si>
+  <si>
+    <t>ECOTOX_exposure_duration_mean_op</t>
+  </si>
+  <si>
+    <t>ECOTOX_exposure_duration_mean</t>
+  </si>
+  <si>
+    <t>ECOTOX_exposure_duration_min_op</t>
+  </si>
+  <si>
+    <t>ECOTOX_exposure_duration_min</t>
+  </si>
+  <si>
+    <t>ECOTOX_exposure_duration_max_op</t>
+  </si>
+  <si>
+    <t>ECOTOX_exposure_duration_max</t>
+  </si>
+  <si>
+    <t>ECOTOX_exposure_duration_comments</t>
+  </si>
+  <si>
+    <t>ECOTOX_study_type</t>
+  </si>
+  <si>
+    <t>ECOTOX_study_type_comments</t>
+  </si>
+  <si>
+    <t>ECOTOX_test_type</t>
+  </si>
+  <si>
+    <t>ECOTOX_test_type_comments</t>
+  </si>
+  <si>
+    <t>ECOTOX_test_location</t>
+  </si>
+  <si>
+    <t>ECOTOX_test_location_comments</t>
+  </si>
+  <si>
+    <t>ECOTOX_test_method</t>
+  </si>
+  <si>
+    <t>ECOTOX_test_method_comments</t>
+  </si>
+  <si>
+    <t>ECOTOX_exposure_type</t>
+  </si>
+  <si>
+    <t>ECOTOX_exposure_type_comments</t>
+  </si>
+  <si>
+    <t>ECOTOX_control_type</t>
+  </si>
+  <si>
+    <t>ECOTOX_control_type_comments</t>
+  </si>
+  <si>
+    <t>ECOTOX_media_type_comments</t>
+  </si>
+  <si>
+    <t>ECOTOX_num_doses_mean_op</t>
+  </si>
+  <si>
+    <t>ECOTOX_num_doses_mean</t>
+  </si>
+  <si>
+    <t>ECOTOX_num_doses_min_op</t>
+  </si>
+  <si>
+    <t>ECOTOX_num_doses_min</t>
+  </si>
+  <si>
+    <t>ECOTOX_num_doses_max_op</t>
+  </si>
+  <si>
+    <t>ECOTOX_num_doses_max</t>
+  </si>
+  <si>
+    <t>ECOTOX_num_doses_comments</t>
+  </si>
+  <si>
+    <t>ECOTOX_other_effect_comments</t>
+  </si>
+  <si>
+    <t>ECOTOX_application_freq_mean_op</t>
+  </si>
+  <si>
+    <t>ECOTOX_application_freq_mean</t>
+  </si>
+  <si>
+    <t>ECOTOX_application_freq_min_op</t>
+  </si>
+  <si>
+    <t>ECOTOX_application_freq_min</t>
+  </si>
+  <si>
+    <t>ECOTOX_application_freq_max_op</t>
+  </si>
+  <si>
+    <t>ECOTOX_application_freq_max</t>
+  </si>
+  <si>
+    <t>ECOTOX_application_freq_unit</t>
+  </si>
+  <si>
+    <t>ECOTOX_application_freq_comments</t>
+  </si>
+  <si>
+    <t>ECOTOX_application_type</t>
+  </si>
+  <si>
+    <t>ECOTOX_application_type_comments</t>
+  </si>
+  <si>
+    <t>ECOTOX_application_rate</t>
+  </si>
+  <si>
+    <t>ECOTOX_application_rate_unit</t>
+  </si>
+  <si>
+    <t>ECOTOX_application_date</t>
+  </si>
+  <si>
+    <t>ECOTOX_application_date_comments</t>
+  </si>
+  <si>
+    <t>ECOTOX_application_season</t>
+  </si>
+  <si>
+    <t>ECOTOX_application_season_comments</t>
+  </si>
+  <si>
+    <t>ECOTOX_subhabitat</t>
+  </si>
+  <si>
+    <t>ECOTOX_subhabitat_description</t>
+  </si>
+  <si>
+    <t>ECOTOX_substrate</t>
+  </si>
+  <si>
+    <t>ECOTOX_substrate_description</t>
+  </si>
+  <si>
+    <t>ECOTOX_water_depth_mean_op</t>
+  </si>
+  <si>
+    <t>ECOTOX_water_depth_mean</t>
+  </si>
+  <si>
+    <t>ECOTOX_water_depth_min_op</t>
+  </si>
+  <si>
+    <t>ECOTOX_water_depth_min</t>
+  </si>
+  <si>
+    <t>ECOTOX_water_depth_max_op</t>
+  </si>
+  <si>
+    <t>ECOTOX_water_depth_max</t>
+  </si>
+  <si>
+    <t>ECOTOX_water_depth_unit</t>
+  </si>
+  <si>
+    <t>ECOTOX_water_depth_comments</t>
+  </si>
+  <si>
+    <t>ECOTOX_geographic_code</t>
+  </si>
+  <si>
+    <t>ECOTOX_geographic_location</t>
+  </si>
+  <si>
+    <t>ECOTOX_latitude</t>
+  </si>
+  <si>
+    <t>ECOTOX_longitude</t>
+  </si>
+  <si>
+    <t>ECOTOX_halflife_mean_op</t>
+  </si>
+  <si>
+    <t>ECOTOX_halflife_mean</t>
+  </si>
+  <si>
+    <t>ECOTOX_halflife_min_op</t>
+  </si>
+  <si>
+    <t>ECOTOX_halflife_min</t>
+  </si>
+  <si>
+    <t>ECOTOX_halflife_max_op</t>
+  </si>
+  <si>
+    <t>ECOTOX_halflife_max</t>
+  </si>
+  <si>
+    <t>ECOTOX_halflife_unit</t>
+  </si>
+  <si>
+    <t>ECOTOX_halflife_comments</t>
+  </si>
+  <si>
+    <t>ECOTOX_tests_additional_comments</t>
+  </si>
+  <si>
+    <t>ECOTOX_tests_created_date</t>
+  </si>
+  <si>
+    <t>ECOTOX_tests_modified_date</t>
+  </si>
+  <si>
+    <t>ECOTOX_published_date</t>
+  </si>
+  <si>
+    <t>ECOTOX_original_test_cas</t>
+  </si>
+  <si>
+    <t>ECOTOX_reference_db</t>
+  </si>
+  <si>
+    <t>ECOTOX_reference_type</t>
+  </si>
+  <si>
+    <t>ECOTOX_author</t>
+  </si>
+  <si>
+    <t>ECOTOX_title</t>
+  </si>
+  <si>
+    <t>ECOTOX_source</t>
+  </si>
+  <si>
+    <t>ECOTOX_year</t>
+  </si>
+  <si>
+    <t>ECOTOX_chemical_name</t>
+  </si>
+  <si>
+    <t>ECOTOX_chemical_group</t>
+  </si>
+  <si>
+    <t>ECOTOX_dtxsid</t>
+  </si>
+  <si>
+    <t>ECOTOX_original_cas_number</t>
+  </si>
+  <si>
+    <t>ECOTOX_common_name</t>
+  </si>
+  <si>
+    <t>ECOTOX_kingdom</t>
+  </si>
+  <si>
+    <t>ECOTOX_phylum_division</t>
+  </si>
+  <si>
+    <t>ECOTOX_subphylum_div</t>
+  </si>
+  <si>
+    <t>ECOTOX_superclass</t>
+  </si>
+  <si>
+    <t>ECOTOX_class</t>
+  </si>
+  <si>
+    <t>ECOTOX_tax_order</t>
+  </si>
+  <si>
+    <t>ECOTOX_family</t>
+  </si>
+  <si>
+    <t>ECOTOX_genus</t>
+  </si>
+  <si>
+    <t>ECOTOX_species</t>
+  </si>
+  <si>
+    <t>ECOTOX_subspecies</t>
+  </si>
+  <si>
+    <t>ECOTOX_variety</t>
+  </si>
+  <si>
+    <t>ECOTOX_Species_group</t>
+  </si>
+  <si>
+    <t>ECOTOX_ncbi_taxid</t>
+  </si>
+  <si>
+    <t>ECOTOX_effect_description</t>
+  </si>
+  <si>
+    <t>ECOTOX_endpoint_description</t>
+  </si>
+  <si>
+    <t>ECOTOX_measurement_description</t>
+  </si>
+  <si>
+    <t>ECOTOX_duration_unit_description_organism</t>
+  </si>
+  <si>
+    <t>ECOTOX_duration_unit_description_study</t>
+  </si>
+  <si>
+    <t>ECOTOX_duration_unit_description_exposure</t>
+  </si>
+  <si>
+    <t>ECOTOX_duration_unit_description_obs</t>
+  </si>
+  <si>
+    <t>ECOTOX_conc1_mean_original</t>
+  </si>
+  <si>
+    <t>ECOTOX_molweight</t>
+  </si>
+  <si>
+    <t>ECOTOX, EFSA</t>
+  </si>
+  <si>
+    <t>EFSA</t>
+  </si>
+  <si>
+    <t>ECOTOX</t>
+  </si>
+  <si>
+    <t>Explanation of column contents in identifiers_v11.csv</t>
+  </si>
+  <si>
+    <t>Explanation of column contents in experimental_dataset_v11.csv</t>
+  </si>
+  <si>
+    <t>Explanation of column contents in QSAR_predictions_v11.csv</t>
+  </si>
+  <si>
+    <t>experiment media (freshwater or salt water)</t>
+  </si>
+  <si>
+    <t>Name of experimental species</t>
+  </si>
+  <si>
+    <t>Exposure duration translated to hours</t>
+  </si>
+  <si>
+    <t>Effect concentration translated to mg per liter</t>
+  </si>
+  <si>
+    <t>Operator of concentration (i.e. = for given, and &gt; or &lt; for limit values)</t>
+  </si>
+  <si>
+    <t>Which database the experimental value originates from</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2060,19 +3140,67 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor theme="1"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="1"/>
+      </right>
       <top/>
       <bottom/>
       <diagonal/>
@@ -2081,7 +3209,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -2090,11 +3218,166 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="11">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="1"/>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Consolas"/>
+        <family val="3"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color theme="1"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <font>
         <strike val="0"/>
@@ -2126,12 +3409,40 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{845CDADC-A613-41BF-A276-F3B54115A158}" name="Tabell1" displayName="Tabell1" ref="B4:G593" totalsRowShown="0">
   <autoFilter ref="B4:G593" xr:uid="{845CDADC-A613-41BF-A276-F3B54115A158}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{F59F3B0F-1377-47B6-B561-79F1347DA351}" name="Column name" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{F59F3B0F-1377-47B6-B561-79F1347DA351}" name="Column name" dataDxfId="10"/>
     <tableColumn id="2" xr3:uid="{DB4F8A55-E6A5-4935-9C3E-B4E5CA5014C1}" name="Data type"/>
     <tableColumn id="3" xr3:uid="{E669FEAE-6560-470C-BB29-92A9396627BF}" name="Primary data source"/>
     <tableColumn id="6" xr3:uid="{7A4570B7-45C5-4913-B89C-9811D32E22D1}" name="Secondary data source"/>
     <tableColumn id="7" xr3:uid="{8872B699-C32D-46CC-A075-5DFFD1E5868A}" name="Endpoint"/>
     <tableColumn id="4" xr3:uid="{9A6030AA-CA20-4D0E-86C7-2115F6FAE834}" name="Description"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{B0D08139-BE40-454D-AE15-83ED71E52BC2}" name="Tabell3" displayName="Tabell3" ref="B4:F331" totalsRowShown="0" headerRowDxfId="0" tableBorderDxfId="2">
+  <autoFilter ref="B4:F331" xr:uid="{B0D08139-BE40-454D-AE15-83ED71E52BC2}"/>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{9F81BABC-FD41-4206-B388-62D1C7050DB3}" name="Column name" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{5F26C6CD-FF5A-430F-9513-49AF64625606}" name="Data type"/>
+    <tableColumn id="3" xr3:uid="{559AC01A-E9BC-4522-8183-63C8C49AD8CF}" name="Primary data source"/>
+    <tableColumn id="4" xr3:uid="{9F35F212-44C5-4CDA-8544-D32AF24C914F}" name="Secondary data source"/>
+    <tableColumn id="5" xr3:uid="{44798B21-644A-490B-88BD-B549C7EECBB4}" name="Description"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{23F9FA92-57D0-4167-A47B-D2AE0C5AB390}" name="Tabell2" displayName="Tabell2" ref="B4:F12" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
+  <autoFilter ref="B4:F12" xr:uid="{23F9FA92-57D0-4167-A47B-D2AE0C5AB390}"/>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{006A9A54-0236-4D68-8B61-77D77E71C1F8}" name="Column name" dataDxfId="9"/>
+    <tableColumn id="2" xr3:uid="{7295C510-40FE-4D9D-A665-E1FDBA31A9E4}" name="Data type" dataDxfId="8"/>
+    <tableColumn id="3" xr3:uid="{FB7C6CFB-761C-4AFB-B851-3D06C515D1E0}" name="Primary data source" dataDxfId="7"/>
+    <tableColumn id="4" xr3:uid="{058F0AC4-4D31-485E-9D6D-66E126E6F626}" name="Secondary data source" dataDxfId="6"/>
+    <tableColumn id="6" xr3:uid="{C4EA5DE4-DEE3-45C3-8D62-72AD7A80C0BA}" name="Description" dataDxfId="5"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2433,11 +3744,79 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D36B2048-821C-47B0-B3EF-7894A4F59796}">
+  <dimension ref="B3:G12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I19" sqref="I19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>659</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>668</v>
+      </c>
+      <c r="E5" t="s">
+        <v>669</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>660</v>
+      </c>
+      <c r="C7" t="s">
+        <v>661</v>
+      </c>
+      <c r="G7" t="s">
+        <v>681</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C8" t="s">
+        <v>662</v>
+      </c>
+      <c r="G8" t="s">
+        <v>665</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C9" t="s">
+        <v>663</v>
+      </c>
+      <c r="G9" t="s">
+        <v>666</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C10" t="s">
+        <v>664</v>
+      </c>
+      <c r="G10" t="s">
+        <v>667</v>
+      </c>
+    </row>
+    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>680</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7448356E-2453-471C-99C8-F0FA41C6DE87}">
   <dimension ref="B2:G593"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2447,12 +3826,12 @@
     <col min="4" max="4" width="21" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="23.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="102.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="121.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
-        <v>659</v>
+        <v>1012</v>
       </c>
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.25">
@@ -2497,7 +3876,7 @@
         <v>210</v>
       </c>
       <c r="D6" t="s">
-        <v>213</v>
+        <v>1007</v>
       </c>
       <c r="E6" t="s">
         <v>221</v>
@@ -13188,4 +14567,2910 @@
     <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF8AE417-D626-486A-87C0-78912EF60B00}">
+  <dimension ref="B2:F331"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="49.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.5703125" customWidth="1"/>
+    <col min="4" max="4" width="23.140625" customWidth="1"/>
+    <col min="5" max="5" width="26.28515625" customWidth="1"/>
+    <col min="6" max="6" width="14.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B2" s="2" t="s">
+        <v>1011</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B4" s="9" t="s">
+        <v>207</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>208</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>215</v>
+      </c>
+      <c r="E4" s="10" t="s">
+        <v>222</v>
+      </c>
+      <c r="F4" s="11" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B5" s="1" t="s">
+        <v>670</v>
+      </c>
+      <c r="C5" t="s">
+        <v>210</v>
+      </c>
+      <c r="D5" t="s">
+        <v>1007</v>
+      </c>
+      <c r="E5" t="s">
+        <v>221</v>
+      </c>
+      <c r="F5" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B6" s="1" t="s">
+        <v>682</v>
+      </c>
+      <c r="C6" t="s">
+        <v>210</v>
+      </c>
+      <c r="D6" t="s">
+        <v>216</v>
+      </c>
+      <c r="E6" t="s">
+        <v>221</v>
+      </c>
+      <c r="F6" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B7" s="1" t="s">
+        <v>683</v>
+      </c>
+      <c r="C7" t="s">
+        <v>210</v>
+      </c>
+      <c r="D7" t="s">
+        <v>1007</v>
+      </c>
+      <c r="F7" t="s">
+        <v>1013</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B8" s="1" t="s">
+        <v>684</v>
+      </c>
+      <c r="C8" t="s">
+        <v>210</v>
+      </c>
+      <c r="D8" t="s">
+        <v>1007</v>
+      </c>
+      <c r="E8" t="s">
+        <v>211</v>
+      </c>
+      <c r="F8" t="s">
+        <v>1014</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B9" s="1" t="s">
+        <v>621</v>
+      </c>
+      <c r="C9" t="s">
+        <v>210</v>
+      </c>
+      <c r="D9" t="s">
+        <v>1007</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B10" s="1" t="s">
+        <v>685</v>
+      </c>
+      <c r="C10" t="s">
+        <v>220</v>
+      </c>
+      <c r="D10" t="s">
+        <v>1007</v>
+      </c>
+      <c r="E10" t="s">
+        <v>211</v>
+      </c>
+      <c r="F10" t="s">
+        <v>1015</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B11" s="1" t="s">
+        <v>686</v>
+      </c>
+      <c r="C11" t="s">
+        <v>220</v>
+      </c>
+      <c r="D11" t="s">
+        <v>1007</v>
+      </c>
+      <c r="E11" t="s">
+        <v>211</v>
+      </c>
+      <c r="F11" t="s">
+        <v>1016</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B12" s="1" t="s">
+        <v>687</v>
+      </c>
+      <c r="C12" t="s">
+        <v>210</v>
+      </c>
+      <c r="D12" t="s">
+        <v>1007</v>
+      </c>
+      <c r="F12" t="s">
+        <v>1017</v>
+      </c>
+    </row>
+    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B13" s="1" t="s">
+        <v>688</v>
+      </c>
+      <c r="C13" t="s">
+        <v>210</v>
+      </c>
+      <c r="D13" t="s">
+        <v>211</v>
+      </c>
+      <c r="F13" t="s">
+        <v>1018</v>
+      </c>
+    </row>
+    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B14" s="1" t="s">
+        <v>689</v>
+      </c>
+      <c r="D14" t="s">
+        <v>1008</v>
+      </c>
+    </row>
+    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B15" s="1" t="s">
+        <v>690</v>
+      </c>
+      <c r="D15" t="s">
+        <v>1008</v>
+      </c>
+    </row>
+    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B16" s="1" t="s">
+        <v>691</v>
+      </c>
+      <c r="D16" t="s">
+        <v>1008</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B17" s="1" t="s">
+        <v>692</v>
+      </c>
+      <c r="D17" t="s">
+        <v>1008</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B18" s="1" t="s">
+        <v>693</v>
+      </c>
+      <c r="D18" t="s">
+        <v>1008</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B19" s="1" t="s">
+        <v>694</v>
+      </c>
+      <c r="D19" t="s">
+        <v>1008</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B20" s="1" t="s">
+        <v>695</v>
+      </c>
+      <c r="D20" t="s">
+        <v>1008</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B21" s="1" t="s">
+        <v>696</v>
+      </c>
+      <c r="D21" t="s">
+        <v>1008</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B22" s="1" t="s">
+        <v>697</v>
+      </c>
+      <c r="D22" t="s">
+        <v>1008</v>
+      </c>
+    </row>
+    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B23" s="1" t="s">
+        <v>698</v>
+      </c>
+      <c r="D23" t="s">
+        <v>1008</v>
+      </c>
+    </row>
+    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B24" s="1" t="s">
+        <v>699</v>
+      </c>
+      <c r="D24" t="s">
+        <v>1008</v>
+      </c>
+    </row>
+    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B25" s="1" t="s">
+        <v>700</v>
+      </c>
+      <c r="D25" t="s">
+        <v>1008</v>
+      </c>
+    </row>
+    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B26" s="1" t="s">
+        <v>701</v>
+      </c>
+      <c r="D26" t="s">
+        <v>1008</v>
+      </c>
+    </row>
+    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B27" s="1" t="s">
+        <v>702</v>
+      </c>
+      <c r="D27" t="s">
+        <v>1008</v>
+      </c>
+    </row>
+    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B28" s="1" t="s">
+        <v>703</v>
+      </c>
+      <c r="D28" t="s">
+        <v>1008</v>
+      </c>
+    </row>
+    <row r="29" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B29" s="1" t="s">
+        <v>704</v>
+      </c>
+      <c r="D29" t="s">
+        <v>1008</v>
+      </c>
+    </row>
+    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B30" s="1" t="s">
+        <v>705</v>
+      </c>
+      <c r="D30" t="s">
+        <v>1008</v>
+      </c>
+    </row>
+    <row r="31" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B31" s="1" t="s">
+        <v>706</v>
+      </c>
+      <c r="D31" t="s">
+        <v>1008</v>
+      </c>
+    </row>
+    <row r="32" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B32" s="1" t="s">
+        <v>707</v>
+      </c>
+      <c r="D32" t="s">
+        <v>1008</v>
+      </c>
+    </row>
+    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B33" s="1" t="s">
+        <v>708</v>
+      </c>
+      <c r="D33" t="s">
+        <v>1008</v>
+      </c>
+    </row>
+    <row r="34" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B34" s="1" t="s">
+        <v>709</v>
+      </c>
+      <c r="D34" t="s">
+        <v>1008</v>
+      </c>
+    </row>
+    <row r="35" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B35" s="1" t="s">
+        <v>710</v>
+      </c>
+      <c r="D35" t="s">
+        <v>1008</v>
+      </c>
+    </row>
+    <row r="36" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B36" s="1" t="s">
+        <v>711</v>
+      </c>
+      <c r="D36" t="s">
+        <v>1008</v>
+      </c>
+    </row>
+    <row r="37" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B37" s="1" t="s">
+        <v>712</v>
+      </c>
+      <c r="D37" t="s">
+        <v>1008</v>
+      </c>
+    </row>
+    <row r="38" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B38" s="1" t="s">
+        <v>713</v>
+      </c>
+      <c r="D38" t="s">
+        <v>1008</v>
+      </c>
+    </row>
+    <row r="39" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B39" s="1" t="s">
+        <v>714</v>
+      </c>
+      <c r="D39" t="s">
+        <v>1008</v>
+      </c>
+    </row>
+    <row r="40" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B40" s="1" t="s">
+        <v>715</v>
+      </c>
+      <c r="D40" t="s">
+        <v>1008</v>
+      </c>
+    </row>
+    <row r="41" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B41" s="1" t="s">
+        <v>716</v>
+      </c>
+      <c r="D41" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="42" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B42" s="1" t="s">
+        <v>717</v>
+      </c>
+      <c r="D42" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="43" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B43" s="1" t="s">
+        <v>718</v>
+      </c>
+      <c r="D43" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="44" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B44" s="1" t="s">
+        <v>719</v>
+      </c>
+      <c r="D44" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="45" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B45" s="1" t="s">
+        <v>720</v>
+      </c>
+      <c r="D45" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="46" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B46" s="1" t="s">
+        <v>721</v>
+      </c>
+      <c r="D46" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="47" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B47" s="1" t="s">
+        <v>722</v>
+      </c>
+      <c r="D47" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="48" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B48" s="1" t="s">
+        <v>723</v>
+      </c>
+      <c r="D48" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="49" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B49" s="1" t="s">
+        <v>724</v>
+      </c>
+      <c r="D49" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="50" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B50" s="1" t="s">
+        <v>725</v>
+      </c>
+      <c r="D50" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="51" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B51" s="1" t="s">
+        <v>726</v>
+      </c>
+      <c r="D51" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="52" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B52" s="1" t="s">
+        <v>727</v>
+      </c>
+      <c r="D52" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="53" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B53" s="1" t="s">
+        <v>728</v>
+      </c>
+      <c r="D53" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="54" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B54" s="1" t="s">
+        <v>729</v>
+      </c>
+      <c r="D54" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="55" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B55" s="1" t="s">
+        <v>730</v>
+      </c>
+      <c r="D55" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="56" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B56" s="1" t="s">
+        <v>731</v>
+      </c>
+      <c r="D56" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="57" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B57" s="1" t="s">
+        <v>732</v>
+      </c>
+      <c r="D57" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="58" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B58" s="1" t="s">
+        <v>733</v>
+      </c>
+      <c r="D58" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="59" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B59" s="1" t="s">
+        <v>734</v>
+      </c>
+      <c r="D59" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="60" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B60" s="1" t="s">
+        <v>735</v>
+      </c>
+      <c r="D60" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="61" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B61" s="1" t="s">
+        <v>736</v>
+      </c>
+      <c r="D61" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="62" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B62" s="1" t="s">
+        <v>737</v>
+      </c>
+      <c r="D62" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="63" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B63" s="1" t="s">
+        <v>738</v>
+      </c>
+      <c r="D63" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="64" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B64" s="1" t="s">
+        <v>739</v>
+      </c>
+      <c r="D64" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="65" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B65" s="1" t="s">
+        <v>740</v>
+      </c>
+      <c r="D65" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="66" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B66" s="1" t="s">
+        <v>741</v>
+      </c>
+      <c r="D66" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="67" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B67" s="1" t="s">
+        <v>742</v>
+      </c>
+      <c r="D67" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="68" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B68" s="1" t="s">
+        <v>743</v>
+      </c>
+      <c r="D68" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="69" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B69" s="1" t="s">
+        <v>744</v>
+      </c>
+      <c r="D69" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="70" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B70" s="1" t="s">
+        <v>745</v>
+      </c>
+      <c r="D70" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="71" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B71" s="1" t="s">
+        <v>746</v>
+      </c>
+      <c r="D71" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="72" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B72" s="1" t="s">
+        <v>747</v>
+      </c>
+      <c r="D72" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="73" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B73" s="1" t="s">
+        <v>748</v>
+      </c>
+      <c r="D73" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="74" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B74" s="1" t="s">
+        <v>749</v>
+      </c>
+      <c r="D74" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="75" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B75" s="1" t="s">
+        <v>750</v>
+      </c>
+      <c r="D75" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="76" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B76" s="1" t="s">
+        <v>751</v>
+      </c>
+      <c r="D76" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="77" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B77" s="1" t="s">
+        <v>752</v>
+      </c>
+      <c r="D77" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="78" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B78" s="1" t="s">
+        <v>753</v>
+      </c>
+      <c r="D78" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="79" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B79" s="1" t="s">
+        <v>754</v>
+      </c>
+      <c r="D79" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="80" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B80" s="1" t="s">
+        <v>755</v>
+      </c>
+      <c r="D80" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="81" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B81" s="1" t="s">
+        <v>756</v>
+      </c>
+      <c r="D81" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="82" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B82" s="1" t="s">
+        <v>757</v>
+      </c>
+      <c r="D82" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="83" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B83" s="1" t="s">
+        <v>758</v>
+      </c>
+      <c r="D83" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="84" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B84" s="1" t="s">
+        <v>759</v>
+      </c>
+      <c r="D84" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="85" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B85" s="1" t="s">
+        <v>760</v>
+      </c>
+      <c r="D85" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="86" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B86" s="1" t="s">
+        <v>761</v>
+      </c>
+      <c r="D86" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="87" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B87" s="1" t="s">
+        <v>762</v>
+      </c>
+      <c r="D87" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="88" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B88" s="1" t="s">
+        <v>763</v>
+      </c>
+      <c r="D88" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="89" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B89" s="1" t="s">
+        <v>764</v>
+      </c>
+      <c r="D89" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="90" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B90" s="1" t="s">
+        <v>765</v>
+      </c>
+      <c r="D90" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="91" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B91" s="1" t="s">
+        <v>766</v>
+      </c>
+      <c r="D91" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="92" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B92" s="1" t="s">
+        <v>767</v>
+      </c>
+      <c r="D92" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="93" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B93" s="1" t="s">
+        <v>768</v>
+      </c>
+      <c r="D93" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="94" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B94" s="1" t="s">
+        <v>769</v>
+      </c>
+      <c r="D94" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="95" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B95" s="1" t="s">
+        <v>770</v>
+      </c>
+      <c r="D95" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="96" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B96" s="1" t="s">
+        <v>771</v>
+      </c>
+      <c r="D96" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="97" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B97" s="1" t="s">
+        <v>772</v>
+      </c>
+      <c r="D97" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="98" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B98" s="1" t="s">
+        <v>773</v>
+      </c>
+      <c r="D98" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="99" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B99" s="1" t="s">
+        <v>774</v>
+      </c>
+      <c r="D99" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="100" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B100" s="1" t="s">
+        <v>775</v>
+      </c>
+      <c r="D100" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="101" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B101" s="1" t="s">
+        <v>776</v>
+      </c>
+      <c r="D101" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="102" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B102" s="1" t="s">
+        <v>777</v>
+      </c>
+      <c r="D102" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="103" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B103" s="1" t="s">
+        <v>778</v>
+      </c>
+      <c r="D103" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="104" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B104" s="1" t="s">
+        <v>779</v>
+      </c>
+      <c r="D104" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="105" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B105" s="1" t="s">
+        <v>780</v>
+      </c>
+      <c r="D105" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="106" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B106" s="1" t="s">
+        <v>781</v>
+      </c>
+      <c r="D106" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="107" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B107" s="1" t="s">
+        <v>782</v>
+      </c>
+      <c r="D107" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="108" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B108" s="1" t="s">
+        <v>783</v>
+      </c>
+      <c r="D108" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="109" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B109" s="1" t="s">
+        <v>784</v>
+      </c>
+      <c r="D109" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="110" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B110" s="1" t="s">
+        <v>785</v>
+      </c>
+      <c r="D110" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="111" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B111" s="1" t="s">
+        <v>786</v>
+      </c>
+      <c r="D111" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="112" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B112" s="1" t="s">
+        <v>787</v>
+      </c>
+      <c r="D112" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="113" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B113" s="1" t="s">
+        <v>788</v>
+      </c>
+      <c r="D113" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="114" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B114" s="1" t="s">
+        <v>789</v>
+      </c>
+      <c r="D114" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="115" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B115" s="1" t="s">
+        <v>790</v>
+      </c>
+      <c r="D115" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="116" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B116" s="1" t="s">
+        <v>791</v>
+      </c>
+      <c r="D116" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="117" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B117" s="1" t="s">
+        <v>792</v>
+      </c>
+      <c r="D117" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="118" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B118" s="1" t="s">
+        <v>793</v>
+      </c>
+      <c r="D118" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="119" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B119" s="1" t="s">
+        <v>794</v>
+      </c>
+      <c r="D119" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="120" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B120" s="1" t="s">
+        <v>795</v>
+      </c>
+      <c r="D120" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="121" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B121" s="1" t="s">
+        <v>796</v>
+      </c>
+      <c r="D121" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="122" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B122" s="1" t="s">
+        <v>797</v>
+      </c>
+      <c r="D122" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="123" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B123" s="1" t="s">
+        <v>798</v>
+      </c>
+      <c r="D123" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="124" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B124" s="1" t="s">
+        <v>799</v>
+      </c>
+      <c r="D124" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="125" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B125" s="1" t="s">
+        <v>800</v>
+      </c>
+      <c r="D125" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="126" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B126" s="1" t="s">
+        <v>801</v>
+      </c>
+      <c r="D126" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="127" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B127" s="1" t="s">
+        <v>802</v>
+      </c>
+      <c r="D127" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="128" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B128" s="1" t="s">
+        <v>803</v>
+      </c>
+      <c r="D128" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="129" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B129" s="1" t="s">
+        <v>804</v>
+      </c>
+      <c r="D129" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="130" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B130" s="1" t="s">
+        <v>805</v>
+      </c>
+      <c r="D130" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="131" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B131" s="1" t="s">
+        <v>806</v>
+      </c>
+      <c r="D131" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="132" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B132" s="1" t="s">
+        <v>807</v>
+      </c>
+      <c r="D132" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="133" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B133" s="1" t="s">
+        <v>808</v>
+      </c>
+      <c r="D133" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="134" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B134" s="1" t="s">
+        <v>809</v>
+      </c>
+      <c r="D134" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="135" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B135" s="1" t="s">
+        <v>810</v>
+      </c>
+      <c r="D135" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="136" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B136" s="1" t="s">
+        <v>811</v>
+      </c>
+      <c r="D136" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="137" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B137" s="1" t="s">
+        <v>812</v>
+      </c>
+      <c r="D137" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="138" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B138" s="1" t="s">
+        <v>813</v>
+      </c>
+      <c r="D138" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="139" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B139" s="1" t="s">
+        <v>814</v>
+      </c>
+      <c r="D139" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="140" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B140" s="1" t="s">
+        <v>815</v>
+      </c>
+      <c r="D140" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="141" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B141" s="1" t="s">
+        <v>816</v>
+      </c>
+      <c r="D141" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="142" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B142" s="1" t="s">
+        <v>817</v>
+      </c>
+      <c r="D142" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="143" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B143" s="1" t="s">
+        <v>818</v>
+      </c>
+      <c r="D143" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="144" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B144" s="1" t="s">
+        <v>819</v>
+      </c>
+      <c r="D144" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="145" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B145" s="1" t="s">
+        <v>820</v>
+      </c>
+      <c r="D145" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="146" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B146" s="1" t="s">
+        <v>821</v>
+      </c>
+      <c r="D146" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="147" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B147" s="1" t="s">
+        <v>822</v>
+      </c>
+      <c r="D147" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="148" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B148" s="1" t="s">
+        <v>823</v>
+      </c>
+      <c r="D148" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="149" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B149" s="1" t="s">
+        <v>824</v>
+      </c>
+      <c r="D149" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="150" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B150" s="1" t="s">
+        <v>825</v>
+      </c>
+      <c r="D150" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="151" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B151" s="1" t="s">
+        <v>826</v>
+      </c>
+      <c r="D151" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="152" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B152" s="1" t="s">
+        <v>827</v>
+      </c>
+      <c r="D152" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="153" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B153" s="1" t="s">
+        <v>828</v>
+      </c>
+      <c r="D153" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="154" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B154" s="1" t="s">
+        <v>829</v>
+      </c>
+      <c r="D154" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="155" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B155" s="1" t="s">
+        <v>830</v>
+      </c>
+      <c r="D155" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="156" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B156" s="1" t="s">
+        <v>831</v>
+      </c>
+      <c r="D156" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="157" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B157" s="1" t="s">
+        <v>832</v>
+      </c>
+      <c r="D157" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="158" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B158" s="1" t="s">
+        <v>833</v>
+      </c>
+      <c r="D158" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="159" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B159" s="1" t="s">
+        <v>834</v>
+      </c>
+      <c r="D159" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="160" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B160" s="1" t="s">
+        <v>835</v>
+      </c>
+      <c r="D160" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="161" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B161" s="1" t="s">
+        <v>836</v>
+      </c>
+      <c r="D161" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="162" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B162" s="1" t="s">
+        <v>837</v>
+      </c>
+      <c r="D162" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="163" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B163" s="1" t="s">
+        <v>838</v>
+      </c>
+      <c r="D163" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="164" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B164" s="1" t="s">
+        <v>839</v>
+      </c>
+      <c r="D164" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="165" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B165" s="1" t="s">
+        <v>840</v>
+      </c>
+      <c r="D165" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="166" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B166" s="1" t="s">
+        <v>841</v>
+      </c>
+      <c r="D166" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="167" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B167" s="1" t="s">
+        <v>842</v>
+      </c>
+      <c r="D167" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="168" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B168" s="1" t="s">
+        <v>843</v>
+      </c>
+      <c r="D168" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="169" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B169" s="1" t="s">
+        <v>844</v>
+      </c>
+      <c r="D169" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="170" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B170" s="1" t="s">
+        <v>845</v>
+      </c>
+      <c r="D170" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="171" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B171" s="1" t="s">
+        <v>846</v>
+      </c>
+      <c r="D171" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="172" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B172" s="1" t="s">
+        <v>847</v>
+      </c>
+      <c r="D172" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="173" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B173" s="1" t="s">
+        <v>848</v>
+      </c>
+      <c r="D173" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="174" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B174" s="1" t="s">
+        <v>849</v>
+      </c>
+      <c r="D174" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="175" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B175" s="1" t="s">
+        <v>850</v>
+      </c>
+      <c r="D175" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="176" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B176" s="1" t="s">
+        <v>851</v>
+      </c>
+      <c r="D176" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="177" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B177" s="1" t="s">
+        <v>852</v>
+      </c>
+      <c r="D177" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="178" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B178" s="1" t="s">
+        <v>853</v>
+      </c>
+      <c r="D178" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="179" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B179" s="1" t="s">
+        <v>854</v>
+      </c>
+      <c r="D179" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="180" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B180" s="1" t="s">
+        <v>855</v>
+      </c>
+      <c r="D180" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="181" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B181" s="1" t="s">
+        <v>856</v>
+      </c>
+      <c r="D181" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="182" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B182" s="1" t="s">
+        <v>857</v>
+      </c>
+      <c r="D182" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="183" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B183" s="1" t="s">
+        <v>858</v>
+      </c>
+      <c r="D183" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="184" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B184" s="1" t="s">
+        <v>859</v>
+      </c>
+      <c r="D184" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="185" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B185" s="1" t="s">
+        <v>860</v>
+      </c>
+      <c r="D185" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="186" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B186" s="1" t="s">
+        <v>861</v>
+      </c>
+      <c r="D186" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="187" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B187" s="1" t="s">
+        <v>862</v>
+      </c>
+      <c r="D187" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="188" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B188" s="1" t="s">
+        <v>863</v>
+      </c>
+      <c r="D188" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="189" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B189" s="1" t="s">
+        <v>864</v>
+      </c>
+      <c r="D189" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="190" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B190" s="1" t="s">
+        <v>865</v>
+      </c>
+      <c r="D190" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="191" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B191" s="1" t="s">
+        <v>866</v>
+      </c>
+      <c r="D191" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="192" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B192" s="1" t="s">
+        <v>867</v>
+      </c>
+      <c r="D192" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="193" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B193" s="1" t="s">
+        <v>868</v>
+      </c>
+      <c r="D193" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="194" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B194" s="1" t="s">
+        <v>869</v>
+      </c>
+      <c r="D194" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="195" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B195" s="1" t="s">
+        <v>870</v>
+      </c>
+      <c r="D195" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="196" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B196" s="1" t="s">
+        <v>871</v>
+      </c>
+      <c r="D196" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="197" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B197" s="1" t="s">
+        <v>872</v>
+      </c>
+      <c r="D197" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="198" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B198" s="1" t="s">
+        <v>873</v>
+      </c>
+      <c r="D198" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="199" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B199" s="1" t="s">
+        <v>874</v>
+      </c>
+      <c r="D199" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="200" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B200" s="1" t="s">
+        <v>875</v>
+      </c>
+      <c r="D200" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="201" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B201" s="1" t="s">
+        <v>876</v>
+      </c>
+      <c r="D201" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="202" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B202" s="1" t="s">
+        <v>877</v>
+      </c>
+      <c r="D202" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="203" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B203" s="1" t="s">
+        <v>878</v>
+      </c>
+      <c r="D203" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="204" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B204" s="1" t="s">
+        <v>879</v>
+      </c>
+      <c r="D204" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="205" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B205" s="1" t="s">
+        <v>880</v>
+      </c>
+      <c r="D205" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="206" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B206" s="1" t="s">
+        <v>881</v>
+      </c>
+      <c r="D206" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="207" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B207" s="1" t="s">
+        <v>882</v>
+      </c>
+      <c r="D207" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="208" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B208" s="1" t="s">
+        <v>883</v>
+      </c>
+      <c r="D208" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="209" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B209" s="1" t="s">
+        <v>884</v>
+      </c>
+      <c r="D209" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="210" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B210" s="1" t="s">
+        <v>885</v>
+      </c>
+      <c r="D210" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="211" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B211" s="1" t="s">
+        <v>886</v>
+      </c>
+      <c r="D211" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="212" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B212" s="1" t="s">
+        <v>887</v>
+      </c>
+      <c r="D212" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="213" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B213" s="1" t="s">
+        <v>888</v>
+      </c>
+      <c r="D213" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="214" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B214" s="1" t="s">
+        <v>889</v>
+      </c>
+      <c r="D214" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="215" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B215" s="1" t="s">
+        <v>890</v>
+      </c>
+      <c r="D215" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="216" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B216" s="1" t="s">
+        <v>891</v>
+      </c>
+      <c r="D216" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="217" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B217" s="1" t="s">
+        <v>892</v>
+      </c>
+      <c r="D217" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="218" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B218" s="1" t="s">
+        <v>893</v>
+      </c>
+      <c r="D218" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="219" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B219" s="1" t="s">
+        <v>894</v>
+      </c>
+      <c r="D219" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="220" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B220" s="1" t="s">
+        <v>895</v>
+      </c>
+      <c r="D220" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="221" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B221" s="1" t="s">
+        <v>896</v>
+      </c>
+      <c r="D221" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="222" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B222" s="1" t="s">
+        <v>897</v>
+      </c>
+      <c r="D222" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="223" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B223" s="1" t="s">
+        <v>898</v>
+      </c>
+      <c r="D223" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="224" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B224" s="1" t="s">
+        <v>899</v>
+      </c>
+      <c r="D224" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="225" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B225" s="1" t="s">
+        <v>900</v>
+      </c>
+      <c r="D225" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="226" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B226" s="1" t="s">
+        <v>901</v>
+      </c>
+      <c r="D226" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="227" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B227" s="1" t="s">
+        <v>902</v>
+      </c>
+      <c r="D227" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="228" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B228" s="1" t="s">
+        <v>903</v>
+      </c>
+      <c r="D228" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="229" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B229" s="1" t="s">
+        <v>904</v>
+      </c>
+      <c r="D229" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="230" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B230" s="1" t="s">
+        <v>905</v>
+      </c>
+      <c r="D230" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="231" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B231" s="1" t="s">
+        <v>906</v>
+      </c>
+      <c r="D231" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="232" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B232" s="1" t="s">
+        <v>907</v>
+      </c>
+      <c r="D232" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="233" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B233" s="1" t="s">
+        <v>908</v>
+      </c>
+      <c r="D233" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="234" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B234" s="1" t="s">
+        <v>909</v>
+      </c>
+      <c r="D234" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="235" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B235" s="1" t="s">
+        <v>910</v>
+      </c>
+      <c r="D235" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="236" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B236" s="1" t="s">
+        <v>911</v>
+      </c>
+      <c r="D236" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="237" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B237" s="1" t="s">
+        <v>912</v>
+      </c>
+      <c r="D237" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="238" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B238" s="1" t="s">
+        <v>913</v>
+      </c>
+      <c r="D238" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="239" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B239" s="1" t="s">
+        <v>914</v>
+      </c>
+      <c r="D239" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="240" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B240" s="1" t="s">
+        <v>915</v>
+      </c>
+      <c r="D240" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="241" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B241" s="1" t="s">
+        <v>916</v>
+      </c>
+      <c r="D241" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="242" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B242" s="1" t="s">
+        <v>917</v>
+      </c>
+      <c r="D242" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="243" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B243" s="1" t="s">
+        <v>918</v>
+      </c>
+      <c r="D243" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="244" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B244" s="1" t="s">
+        <v>919</v>
+      </c>
+      <c r="D244" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="245" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B245" s="1" t="s">
+        <v>920</v>
+      </c>
+      <c r="D245" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="246" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B246" s="1" t="s">
+        <v>921</v>
+      </c>
+      <c r="D246" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="247" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B247" s="1" t="s">
+        <v>922</v>
+      </c>
+      <c r="D247" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="248" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B248" s="1" t="s">
+        <v>923</v>
+      </c>
+      <c r="D248" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="249" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B249" s="1" t="s">
+        <v>924</v>
+      </c>
+      <c r="D249" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="250" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B250" s="1" t="s">
+        <v>925</v>
+      </c>
+      <c r="D250" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="251" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B251" s="1" t="s">
+        <v>926</v>
+      </c>
+      <c r="D251" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="252" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B252" s="1" t="s">
+        <v>927</v>
+      </c>
+      <c r="D252" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="253" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B253" s="1" t="s">
+        <v>928</v>
+      </c>
+      <c r="D253" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="254" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B254" s="1" t="s">
+        <v>929</v>
+      </c>
+      <c r="D254" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="255" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B255" s="1" t="s">
+        <v>930</v>
+      </c>
+      <c r="D255" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="256" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B256" s="1" t="s">
+        <v>931</v>
+      </c>
+      <c r="D256" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="257" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B257" s="1" t="s">
+        <v>932</v>
+      </c>
+      <c r="D257" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="258" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B258" s="1" t="s">
+        <v>933</v>
+      </c>
+      <c r="D258" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="259" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B259" s="1" t="s">
+        <v>934</v>
+      </c>
+      <c r="D259" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="260" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B260" s="1" t="s">
+        <v>935</v>
+      </c>
+      <c r="D260" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="261" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B261" s="1" t="s">
+        <v>936</v>
+      </c>
+      <c r="D261" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="262" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B262" s="1" t="s">
+        <v>937</v>
+      </c>
+      <c r="D262" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="263" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B263" s="1" t="s">
+        <v>938</v>
+      </c>
+      <c r="D263" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="264" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B264" s="1" t="s">
+        <v>939</v>
+      </c>
+      <c r="D264" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="265" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B265" s="1" t="s">
+        <v>940</v>
+      </c>
+      <c r="D265" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="266" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B266" s="1" t="s">
+        <v>941</v>
+      </c>
+      <c r="D266" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="267" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B267" s="1" t="s">
+        <v>942</v>
+      </c>
+      <c r="D267" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="268" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B268" s="1" t="s">
+        <v>943</v>
+      </c>
+      <c r="D268" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="269" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B269" s="1" t="s">
+        <v>944</v>
+      </c>
+      <c r="D269" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="270" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B270" s="1" t="s">
+        <v>945</v>
+      </c>
+      <c r="D270" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="271" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B271" s="1" t="s">
+        <v>946</v>
+      </c>
+      <c r="D271" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="272" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B272" s="1" t="s">
+        <v>947</v>
+      </c>
+      <c r="D272" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="273" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B273" s="1" t="s">
+        <v>948</v>
+      </c>
+      <c r="D273" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="274" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B274" s="1" t="s">
+        <v>949</v>
+      </c>
+      <c r="D274" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="275" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B275" s="1" t="s">
+        <v>950</v>
+      </c>
+      <c r="D275" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="276" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B276" s="1" t="s">
+        <v>951</v>
+      </c>
+      <c r="D276" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="277" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B277" s="1" t="s">
+        <v>952</v>
+      </c>
+      <c r="D277" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="278" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B278" s="1" t="s">
+        <v>953</v>
+      </c>
+      <c r="D278" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="279" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B279" s="1" t="s">
+        <v>954</v>
+      </c>
+      <c r="D279" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="280" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B280" s="1" t="s">
+        <v>955</v>
+      </c>
+      <c r="D280" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="281" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B281" s="1" t="s">
+        <v>956</v>
+      </c>
+      <c r="D281" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="282" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B282" s="1" t="s">
+        <v>957</v>
+      </c>
+      <c r="D282" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="283" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B283" s="1" t="s">
+        <v>958</v>
+      </c>
+      <c r="D283" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="284" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B284" s="1" t="s">
+        <v>959</v>
+      </c>
+      <c r="D284" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="285" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B285" s="1" t="s">
+        <v>960</v>
+      </c>
+      <c r="D285" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="286" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B286" s="1" t="s">
+        <v>961</v>
+      </c>
+      <c r="D286" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="287" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B287" s="1" t="s">
+        <v>962</v>
+      </c>
+      <c r="D287" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="288" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B288" s="1" t="s">
+        <v>963</v>
+      </c>
+      <c r="D288" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="289" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B289" s="1" t="s">
+        <v>964</v>
+      </c>
+      <c r="D289" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="290" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B290" s="1" t="s">
+        <v>965</v>
+      </c>
+      <c r="D290" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="291" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B291" s="1" t="s">
+        <v>966</v>
+      </c>
+      <c r="D291" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="292" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B292" s="1" t="s">
+        <v>967</v>
+      </c>
+      <c r="D292" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="293" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B293" s="1" t="s">
+        <v>968</v>
+      </c>
+      <c r="D293" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="294" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B294" s="1" t="s">
+        <v>969</v>
+      </c>
+      <c r="D294" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="295" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B295" s="1" t="s">
+        <v>970</v>
+      </c>
+      <c r="D295" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="296" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B296" s="1" t="s">
+        <v>971</v>
+      </c>
+      <c r="D296" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="297" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B297" s="1" t="s">
+        <v>972</v>
+      </c>
+      <c r="D297" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="298" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B298" s="1" t="s">
+        <v>973</v>
+      </c>
+      <c r="D298" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="299" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B299" s="1" t="s">
+        <v>974</v>
+      </c>
+      <c r="D299" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="300" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B300" s="1" t="s">
+        <v>975</v>
+      </c>
+      <c r="D300" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="301" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B301" s="1" t="s">
+        <v>976</v>
+      </c>
+      <c r="D301" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="302" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B302" s="1" t="s">
+        <v>977</v>
+      </c>
+      <c r="D302" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="303" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B303" s="1" t="s">
+        <v>978</v>
+      </c>
+      <c r="D303" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="304" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B304" s="1" t="s">
+        <v>979</v>
+      </c>
+      <c r="D304" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="305" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B305" s="1" t="s">
+        <v>980</v>
+      </c>
+      <c r="D305" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="306" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B306" s="1" t="s">
+        <v>981</v>
+      </c>
+      <c r="D306" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="307" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B307" s="1" t="s">
+        <v>982</v>
+      </c>
+      <c r="D307" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="308" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B308" s="1" t="s">
+        <v>983</v>
+      </c>
+      <c r="D308" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="309" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B309" s="1" t="s">
+        <v>984</v>
+      </c>
+      <c r="D309" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="310" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B310" s="1" t="s">
+        <v>985</v>
+      </c>
+      <c r="D310" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="311" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B311" s="1" t="s">
+        <v>986</v>
+      </c>
+      <c r="D311" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="312" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B312" s="1" t="s">
+        <v>987</v>
+      </c>
+      <c r="D312" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="313" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B313" s="1" t="s">
+        <v>988</v>
+      </c>
+      <c r="D313" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="314" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B314" s="1" t="s">
+        <v>989</v>
+      </c>
+      <c r="D314" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="315" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B315" s="1" t="s">
+        <v>990</v>
+      </c>
+      <c r="D315" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="316" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B316" s="1" t="s">
+        <v>991</v>
+      </c>
+      <c r="D316" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="317" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B317" s="1" t="s">
+        <v>992</v>
+      </c>
+      <c r="D317" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="318" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B318" s="1" t="s">
+        <v>993</v>
+      </c>
+      <c r="D318" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="319" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B319" s="1" t="s">
+        <v>994</v>
+      </c>
+      <c r="D319" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="320" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B320" s="1" t="s">
+        <v>995</v>
+      </c>
+      <c r="D320" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="321" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B321" s="1" t="s">
+        <v>996</v>
+      </c>
+      <c r="D321" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="322" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B322" s="1" t="s">
+        <v>997</v>
+      </c>
+      <c r="D322" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="323" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B323" s="1" t="s">
+        <v>998</v>
+      </c>
+      <c r="D323" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="324" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B324" s="1" t="s">
+        <v>999</v>
+      </c>
+      <c r="D324" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="325" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B325" s="1" t="s">
+        <v>1000</v>
+      </c>
+      <c r="D325" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="326" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B326" s="1" t="s">
+        <v>1001</v>
+      </c>
+      <c r="D326" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="327" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B327" s="1" t="s">
+        <v>1002</v>
+      </c>
+      <c r="D327" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="328" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B328" s="1" t="s">
+        <v>1003</v>
+      </c>
+      <c r="D328" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="329" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B329" s="1" t="s">
+        <v>1004</v>
+      </c>
+      <c r="D329" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="330" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B330" s="1" t="s">
+        <v>1005</v>
+      </c>
+      <c r="D330" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="331" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B331" s="1" t="s">
+        <v>1006</v>
+      </c>
+      <c r="D331" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8208BF41-A565-4F27-9C81-D5C742C21AC6}">
+  <dimension ref="B2:F12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="63.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" customWidth="1"/>
+    <col min="4" max="4" width="20.5703125" customWidth="1"/>
+    <col min="5" max="5" width="22.85546875" customWidth="1"/>
+    <col min="6" max="6" width="97.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B2" s="2" t="s">
+        <v>1010</v>
+      </c>
+    </row>
+    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B3" s="2"/>
+    </row>
+    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B4" s="6" t="s">
+        <v>207</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>208</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>215</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>222</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B5" s="8" t="s">
+        <v>670</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>210</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>213</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>221</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B6" s="8" t="s">
+        <v>671</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>210</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>216</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>221</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B7" s="8" t="s">
+        <v>672</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>210</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>216</v>
+      </c>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B8" s="8" t="s">
+        <v>673</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>210</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>216</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>221</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B9" s="8" t="s">
+        <v>677</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>678</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>211</v>
+      </c>
+      <c r="E9" s="7"/>
+      <c r="F9" s="4" t="s">
+        <v>679</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B10" s="8" t="s">
+        <v>674</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>220</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>221</v>
+      </c>
+      <c r="E10" s="7"/>
+      <c r="F10" s="7" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B11" s="8" t="s">
+        <v>675</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>210</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>211</v>
+      </c>
+      <c r="E11" s="7"/>
+      <c r="F11" s="7" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B12" s="8" t="s">
+        <v>676</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>210</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>221</v>
+      </c>
+      <c r="E12" s="7"/>
+      <c r="F12" s="7" t="s">
+        <v>225</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>